<commit_message>
Added : Excel file and Config Properties File
</commit_message>
<xml_diff>
--- a/KeywordDrivenFramework/src/main/resources/Repository/LoginTestKeywordData.xlsx
+++ b/KeywordDrivenFramework/src/main/resources/Repository/LoginTestKeywordData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="15330" windowHeight="3450" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="16245" windowHeight="6615" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="LoginTestData" sheetId="1" r:id="rId1"/>
@@ -619,7 +619,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -627,22 +627,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="18.140625" customWidth="1"/>
-    <col min="2" max="2" width="49.5703125" customWidth="1"/>
+    <col min="2" max="2" width="37.85546875" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" customWidth="1"/>
     <col min="4" max="4" width="24" customWidth="1"/>
     <col min="5" max="1025" width="11.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -656,7 +656,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -670,7 +670,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:5">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -684,7 +684,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:5">
       <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
@@ -698,7 +698,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:5">
       <c r="A5" s="2" t="s">
         <v>14</v>
       </c>
@@ -712,7 +712,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:5">
       <c r="A6" s="2" t="s">
         <v>16</v>
       </c>
@@ -726,7 +726,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:5">
       <c r="A7" s="2" t="s">
         <v>18</v>
       </c>
@@ -739,6 +739,7 @@
       <c r="D7" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="E7" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>